<commit_message>
risk assessment updated and presentation created
</commit_message>
<xml_diff>
--- a/documentation/IMS - Risk Assessment.xlsx
+++ b/documentation/IMS - Risk Assessment.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sanchay/Downloads/IMS_Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sanchay/Documents/GitHub/QA_IMS_Project/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7696601B-5B08-0541-96A6-0E54DD8038A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{351D53CD-819D-3649-9176-FCD2AC54266C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5060" yWindow="1560" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IMS - Risk Assessment" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="48">
   <si>
     <t>Risks</t>
   </si>
@@ -151,6 +151,30 @@
   </si>
   <si>
     <t>Regular breaks from work and stay well hydrated to prevent exhuastation and dehydartion.</t>
+  </si>
+  <si>
+    <t>This proved to be a main issue in th eproject progression. Implementing the features required for an MVP proved to be difficult and time consuming with the lack of pragramming experience.</t>
+  </si>
+  <si>
+    <t>Product did not meet the MVP due to pragramming experience rather than comprehension of the project objective.</t>
+  </si>
+  <si>
+    <t>Was able to manage time well. Using sprints to track progress but somefeautures were taking  too long to implement therefore skipped then cycled back to if there was time.</t>
+  </si>
+  <si>
+    <t>This was a major issue during the week so I chose to avoid the problem and do my work at a friends.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No unplanned absences </t>
+  </si>
+  <si>
+    <t>No hardware filure and changes were regularly comitted and pushed to the remote repository.</t>
+  </si>
+  <si>
+    <t>Test failed to meet 80%. Lack of mockito testing knowledge prevented me from implementing tests on ItemController, OrderController and OrderItems Controller.</t>
+  </si>
+  <si>
+    <t>No hospitalisations .</t>
   </si>
 </sst>
 </file>
@@ -359,7 +383,73 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -376,72 +466,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -771,8 +795,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -792,26 +816,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="15" t="s">
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" s="16"/>
-      <c r="I1" s="15" t="s">
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="38"/>
+      <c r="I1" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="14" t="s">
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
+      <c r="L1" s="35" t="s">
         <v>16</v>
       </c>
     </row>
@@ -849,7 +873,7 @@
       <c r="K2" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="L2" s="39"/>
+      <c r="L2" s="36"/>
     </row>
     <row r="3" spans="1:12" s="9" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7">
@@ -861,14 +885,14 @@
       <c r="C3" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="28">
+      <c r="D3" s="22">
         <v>3</v>
       </c>
-      <c r="E3" s="23">
-        <v>5</v>
-      </c>
-      <c r="F3" s="30">
-        <f t="shared" ref="F3:F18" si="0">D3*E3</f>
+      <c r="E3" s="17">
+        <v>5</v>
+      </c>
+      <c r="F3" s="24">
+        <f t="shared" ref="F3:F9" si="0">D3*E3</f>
         <v>15</v>
       </c>
       <c r="G3" s="9" t="s">
@@ -877,35 +901,37 @@
       <c r="H3" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="21">
-        <v>1</v>
-      </c>
-      <c r="J3" s="23">
-        <v>5</v>
-      </c>
-      <c r="K3" s="23">
+      <c r="I3" s="15">
+        <v>1</v>
+      </c>
+      <c r="J3" s="17">
+        <v>5</v>
+      </c>
+      <c r="K3" s="17">
         <f>I3*J3</f>
         <v>5</v>
       </c>
-      <c r="L3" s="38"/>
-    </row>
-    <row r="4" spans="1:12" s="26" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="24">
+      <c r="L3" s="32" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" s="20" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="18">
         <v>2</v>
       </c>
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="19" t="s">
         <v>19</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="21">
-        <v>1</v>
-      </c>
-      <c r="E4" s="23">
-        <v>5</v>
-      </c>
-      <c r="F4" s="23">
+      <c r="D4" s="15">
+        <v>1</v>
+      </c>
+      <c r="E4" s="17">
+        <v>5</v>
+      </c>
+      <c r="F4" s="17">
         <f>D4*E4</f>
         <v>5</v>
       </c>
@@ -915,17 +941,19 @@
       <c r="H4" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="I4" s="21">
-        <v>1</v>
-      </c>
-      <c r="J4" s="21">
-        <v>1</v>
-      </c>
-      <c r="K4" s="21">
+      <c r="I4" s="15">
+        <v>1</v>
+      </c>
+      <c r="J4" s="15">
+        <v>1</v>
+      </c>
+      <c r="K4" s="15">
         <f>I4*J4</f>
         <v>1</v>
       </c>
-      <c r="L4" s="40"/>
+      <c r="L4" s="33" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="5" spans="1:12" s="9" customFormat="1" ht="82" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="7">
@@ -937,13 +965,13 @@
       <c r="C5" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="28">
+      <c r="D5" s="22">
         <v>3</v>
       </c>
-      <c r="E5" s="23">
-        <v>5</v>
-      </c>
-      <c r="F5" s="30">
+      <c r="E5" s="17">
+        <v>5</v>
+      </c>
+      <c r="F5" s="24">
         <f t="shared" ref="F5" si="1">D5*E5</f>
         <v>15</v>
       </c>
@@ -953,20 +981,22 @@
       <c r="H5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="21">
-        <v>1</v>
-      </c>
-      <c r="J5" s="23">
-        <v>5</v>
-      </c>
-      <c r="K5" s="23">
+      <c r="I5" s="15">
+        <v>1</v>
+      </c>
+      <c r="J5" s="17">
+        <v>5</v>
+      </c>
+      <c r="K5" s="17">
         <f>I5*J5</f>
         <v>5</v>
       </c>
-      <c r="L5" s="38"/>
+      <c r="L5" s="32" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="6" spans="1:12" s="9" customFormat="1" ht="103" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="24">
+      <c r="A6" s="18">
         <v>4</v>
       </c>
       <c r="B6" s="8" t="s">
@@ -975,13 +1005,13 @@
       <c r="C6" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="28">
+      <c r="D6" s="22">
         <v>3</v>
       </c>
-      <c r="E6" s="23">
-        <v>5</v>
-      </c>
-      <c r="F6" s="30">
+      <c r="E6" s="17">
+        <v>5</v>
+      </c>
+      <c r="F6" s="24">
         <f t="shared" ref="F6" si="2">D6*E6</f>
         <v>15</v>
       </c>
@@ -991,17 +1021,19 @@
       <c r="H6" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="I6" s="21">
-        <v>1</v>
-      </c>
-      <c r="J6" s="21">
-        <v>1</v>
-      </c>
-      <c r="K6" s="21">
+      <c r="I6" s="15">
+        <v>1</v>
+      </c>
+      <c r="J6" s="15">
+        <v>1</v>
+      </c>
+      <c r="K6" s="15">
         <f>I6*J6</f>
         <v>1</v>
       </c>
-      <c r="L6" s="38"/>
+      <c r="L6" s="32" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="7" spans="1:12" s="9" customFormat="1" ht="73" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="7">
@@ -1013,13 +1045,13 @@
       <c r="C7" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="31">
+      <c r="D7" s="25">
         <v>2</v>
       </c>
-      <c r="E7" s="33">
+      <c r="E7" s="27">
         <v>4</v>
       </c>
-      <c r="F7" s="35">
+      <c r="F7" s="29">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
@@ -1029,21 +1061,23 @@
       <c r="H7" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="I7" s="31">
+      <c r="I7" s="25">
         <v>2</v>
       </c>
-      <c r="J7" s="33">
+      <c r="J7" s="27">
         <v>4</v>
       </c>
-      <c r="K7" s="35">
+      <c r="K7" s="29">
         <f t="shared" ref="K7" si="3">I7*J7</f>
         <v>8</v>
       </c>
-      <c r="L7" s="38"/>
+      <c r="L7" s="32" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="8" spans="1:12" s="9" customFormat="1" ht="118" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="7">
-        <f t="shared" ref="A6:A18" si="4">A7+1</f>
+        <f t="shared" ref="A8:A10" si="4">A7+1</f>
         <v>6</v>
       </c>
       <c r="B8" s="8" t="s">
@@ -1052,13 +1086,13 @@
       <c r="C8" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="33">
+      <c r="D8" s="27">
         <v>4</v>
       </c>
-      <c r="E8" s="23">
-        <v>5</v>
-      </c>
-      <c r="F8" s="37">
+      <c r="E8" s="17">
+        <v>5</v>
+      </c>
+      <c r="F8" s="31">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
@@ -1068,17 +1102,19 @@
       <c r="H8" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="I8" s="31">
+      <c r="I8" s="25">
         <v>2</v>
       </c>
-      <c r="J8" s="21">
-        <v>1</v>
-      </c>
-      <c r="K8" s="21">
+      <c r="J8" s="15">
+        <v>1</v>
+      </c>
+      <c r="K8" s="15">
         <f>I8*J8</f>
         <v>2</v>
       </c>
-      <c r="L8" s="38"/>
+      <c r="L8" s="32" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="9" spans="1:12" s="9" customFormat="1" ht="102" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7">
@@ -1091,13 +1127,13 @@
       <c r="C9" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="D9" s="28">
+      <c r="D9" s="22">
         <v>3</v>
       </c>
-      <c r="E9" s="23">
-        <v>5</v>
-      </c>
-      <c r="F9" s="30">
+      <c r="E9" s="17">
+        <v>5</v>
+      </c>
+      <c r="F9" s="24">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
@@ -1107,17 +1143,19 @@
       <c r="H9" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="I9" s="31">
+      <c r="I9" s="25">
         <v>2</v>
       </c>
-      <c r="J9" s="31">
+      <c r="J9" s="25">
         <v>2</v>
       </c>
-      <c r="K9" s="33">
-        <f t="shared" ref="K5:K18" si="5">I9*J9</f>
+      <c r="K9" s="27">
+        <f t="shared" ref="K9" si="5">I9*J9</f>
         <v>4</v>
       </c>
-      <c r="L9" s="38"/>
+      <c r="L9" s="32" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="10" spans="1:12" s="9" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="7">
@@ -1130,13 +1168,13 @@
       <c r="C10" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="21">
-        <v>1</v>
-      </c>
-      <c r="E10" s="23">
-        <v>5</v>
-      </c>
-      <c r="F10" s="23">
+      <c r="D10" s="15">
+        <v>1</v>
+      </c>
+      <c r="E10" s="17">
+        <v>5</v>
+      </c>
+      <c r="F10" s="17">
         <f>D10*E10</f>
         <v>5</v>
       </c>
@@ -1146,17 +1184,19 @@
       <c r="H10" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="I10" s="21">
-        <v>1</v>
-      </c>
-      <c r="J10" s="21">
-        <v>1</v>
-      </c>
-      <c r="K10" s="21">
+      <c r="I10" s="15">
+        <v>1</v>
+      </c>
+      <c r="J10" s="15">
+        <v>1</v>
+      </c>
+      <c r="K10" s="15">
         <f>I10*J10</f>
         <v>1</v>
       </c>
-      <c r="L10" s="38"/>
+      <c r="L10" s="32" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="11" spans="1:12" s="9" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="7"/>
@@ -1170,7 +1210,7 @@
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
-      <c r="L11" s="38"/>
+      <c r="L11" s="32"/>
     </row>
     <row r="12" spans="1:12" s="9" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="7"/>
@@ -1184,7 +1224,7 @@
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
-      <c r="L12" s="38"/>
+      <c r="L12" s="32"/>
     </row>
     <row r="13" spans="1:12" s="9" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="7"/>
@@ -1198,7 +1238,7 @@
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
-      <c r="L13" s="38"/>
+      <c r="L13" s="32"/>
     </row>
     <row r="14" spans="1:12" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="7"/>
@@ -1212,7 +1252,7 @@
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
-      <c r="L14" s="41"/>
+      <c r="L14" s="34"/>
     </row>
     <row r="15" spans="1:12" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="7"/>
@@ -1226,7 +1266,7 @@
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
-      <c r="L15" s="41"/>
+      <c r="L15" s="34"/>
     </row>
     <row r="16" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="7"/>
@@ -1240,7 +1280,7 @@
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
-      <c r="L16" s="41"/>
+      <c r="L16" s="34"/>
     </row>
     <row r="17" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="7"/>
@@ -1254,7 +1294,7 @@
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
-      <c r="L17" s="41"/>
+      <c r="L17" s="34"/>
     </row>
     <row r="18" spans="1:12" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="7"/>
@@ -1268,7 +1308,7 @@
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
-      <c r="L18" s="41"/>
+      <c r="L18" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1296,13 +1336,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="39" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="13">
         <v>5</v>
       </c>
-      <c r="C1" s="22">
+      <c r="C1" s="16">
         <f t="shared" ref="C1:D1" si="0">$B1*C$6</f>
         <v>5</v>
       </c>
@@ -1310,11 +1350,11 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="E1" s="29">
+      <c r="E1" s="23">
         <f>$B1*E$6</f>
         <v>15</v>
       </c>
-      <c r="F1" s="36">
+      <c r="F1" s="30">
         <f t="shared" ref="F1:G5" si="1">$B1*F$6</f>
         <v>20</v>
       </c>
@@ -1324,7 +1364,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="17"/>
+      <c r="A2" s="39"/>
       <c r="B2" s="13">
         <v>4</v>
       </c>
@@ -1332,7 +1372,7 @@
         <f t="shared" ref="C2:E5" si="2">$B2*C$6</f>
         <v>4</v>
       </c>
-      <c r="D2" s="34">
+      <c r="D2" s="28">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
@@ -1350,7 +1390,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="17"/>
+      <c r="A3" s="39"/>
       <c r="B3" s="13">
         <v>3</v>
       </c>
@@ -1376,15 +1416,15 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="17"/>
+      <c r="A4" s="39"/>
       <c r="B4" s="13">
         <v>2</v>
       </c>
-      <c r="C4" s="22">
+      <c r="C4" s="16">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="D4" s="32">
+      <c r="D4" s="26">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
@@ -1402,23 +1442,23 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="17"/>
+      <c r="A5" s="39"/>
       <c r="B5" s="13">
         <v>1</v>
       </c>
-      <c r="C5" s="20">
+      <c r="C5" s="14">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="D5" s="32">
+      <c r="D5" s="26">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="E5" s="27">
+      <c r="E5" s="21">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="F5" s="22">
+      <c r="F5" s="16">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
@@ -1428,7 +1468,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="17"/>
+      <c r="A6" s="39"/>
       <c r="B6" s="13"/>
       <c r="C6" s="4">
         <v>1</v>
@@ -1447,14 +1487,14 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
+      <c r="B7" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="41"/>
+      <c r="D7" s="41"/>
+      <c r="E7" s="41"/>
+      <c r="F7" s="41"/>
+      <c r="G7" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>